<commit_message>
Implement expense management features: add AddExpenseForm, ExpenseList, and ExpenseOverview components; update Expense page to handle expense addition, deletion, and downloading; enhance API paths for expenses and incomes; add expense line chart data preparation utility.
</commit_message>
<xml_diff>
--- a/backend/incomes_details.xlsx
+++ b/backend/incomes_details.xlsx
@@ -397,13 +397,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Source</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>salary</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2" t="str">
+        <v>6/9/2025</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>toy</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="str">
+        <v>13/8/2025</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>girlfriend</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4" t="str">
+        <v>13/8/2025</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>bakchodi</v>
+      </c>
+      <c r="B5">
+        <v>2000</v>
+      </c>
+      <c r="C5" t="str">
+        <v>13/8/2025</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>freelance</v>
+      </c>
+      <c r="B6">
+        <v>679</v>
+      </c>
+      <c r="C6" t="str">
+        <v>12/8/2025</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Avacado</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" t="str">
+        <v>12/8/2025</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>sold car</v>
+      </c>
+      <c r="B8">
+        <v>5000</v>
+      </c>
+      <c r="C8" t="str">
+        <v>7/7/2025</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>abhayawas@gmail.com</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="str">
+        <v>3/6/2025</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>john@example.com</v>
+      </c>
+      <c r="B10">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="str">
+        <v>3/5/2024</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented the new features- advanced analytics
</commit_message>
<xml_diff>
--- a/backend/incomes_details.xlsx
+++ b/backend/incomes_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -481,40 +481,29 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>sold car</v>
+        <v>abhayawas@gmail.com</v>
       </c>
       <c r="B8">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C8" t="str">
-        <v>7/7/2025</v>
+        <v>3/6/2025</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>abhayawas@gmail.com</v>
+        <v>john@example.com</v>
       </c>
       <c r="B9">
         <v>1000</v>
       </c>
       <c r="C9" t="str">
-        <v>3/6/2025</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>john@example.com</v>
-      </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10" t="str">
         <v>3/5/2024</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>